<commit_message>
update customer and artisan
</commit_message>
<xml_diff>
--- a/Artisan Backend Timeline.xlsx
+++ b/Artisan Backend Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\locale\ly\projects\artisan-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2250BA0-3A17-4AC5-A243-BFCECC65CE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49C5D43-CC2A-4807-97DD-2C2D10CF97D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7352EEA0-E213-4B45-A5B2-9E24555BD19A}"/>
   </bookViews>
@@ -1045,18 +1045,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1066,11 +1054,23 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1397,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EC11CA-85A1-4736-9D8D-54DA1C1DECD6}">
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="L84" sqref="L84"/>
+    <sheetView tabSelected="1" topLeftCell="E43" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1427,40 +1427,40 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="H3" s="35" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="H3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="37"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="33"/>
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
       <c r="H4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="33" t="s">
+      <c r="I4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="35"/>
       <c r="N4" t="s">
         <v>43</v>
       </c>
@@ -1469,10 +1469,10 @@
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="39"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
@@ -1482,10 +1482,10 @@
       <c r="H5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="39"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="15" t="s">
         <v>3</v>
       </c>
@@ -1753,12 +1753,12 @@
       <c r="A24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="35"/>
       <c r="H24" s="17" t="s">
         <v>39</v>
       </c>
@@ -1832,12 +1832,12 @@
       <c r="H31" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I31" s="33" t="s">
+      <c r="I31" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="35"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
@@ -1866,6 +1866,7 @@
       <c r="K33" s="5" t="s">
         <v>220</v>
       </c>
+      <c r="L33" s="22"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
@@ -1889,6 +1890,7 @@
       <c r="J35" s="1">
         <v>44639</v>
       </c>
+      <c r="L35" s="22"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
@@ -1951,10 +1953,10 @@
       <c r="H41" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="I41" s="31">
+      <c r="I41" s="38">
         <v>44641</v>
       </c>
-      <c r="J41" s="31">
+      <c r="J41" s="38">
         <v>44642</v>
       </c>
       <c r="L41" s="22"/>
@@ -1966,8 +1968,8 @@
       <c r="H42" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="38"/>
       <c r="L42" s="22"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
@@ -1977,8 +1979,8 @@
       <c r="H43" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
@@ -1987,8 +1989,8 @@
       <c r="H44" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="I44" s="31"/>
-      <c r="J44" s="31"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="38"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
@@ -2000,10 +2002,10 @@
       <c r="H45" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="I45" s="31">
+      <c r="I45" s="38">
         <v>44644</v>
       </c>
-      <c r="J45" s="31">
+      <c r="J45" s="38">
         <v>44645</v>
       </c>
       <c r="L45" s="22"/>
@@ -2015,8 +2017,8 @@
       <c r="H46" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
       <c r="L46" s="22"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
@@ -2026,8 +2028,8 @@
       <c r="H47" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="38"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
@@ -2036,8 +2038,8 @@
       <c r="H48" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="I48" s="31"/>
-      <c r="J48" s="31"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="38"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
@@ -2046,10 +2048,10 @@
       <c r="H49" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="I49" s="31">
+      <c r="I49" s="38">
         <v>44646</v>
       </c>
-      <c r="J49" s="31">
+      <c r="J49" s="38">
         <v>44648</v>
       </c>
     </row>
@@ -2060,8 +2062,8 @@
       <c r="H50" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="I50" s="31"/>
-      <c r="J50" s="31"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="38"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="17" t="s">
@@ -2078,10 +2080,10 @@
       <c r="H52" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="I52" s="31">
+      <c r="I52" s="38">
         <v>44652</v>
       </c>
-      <c r="J52" s="31">
+      <c r="J52" s="38">
         <v>44655</v>
       </c>
     </row>
@@ -2092,8 +2094,8 @@
       <c r="H53" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="I53" s="31"/>
-      <c r="J53" s="31"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="38"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="17" t="s">
@@ -2102,8 +2104,8 @@
       <c r="H54" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="I54" s="31"/>
-      <c r="J54" s="31"/>
+      <c r="I54" s="38"/>
+      <c r="J54" s="38"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="17" t="s">
@@ -2123,10 +2125,10 @@
       <c r="H56" t="s">
         <v>60</v>
       </c>
-      <c r="I56" s="31">
+      <c r="I56" s="38">
         <v>44657</v>
       </c>
-      <c r="J56" s="31">
+      <c r="J56" s="38">
         <v>44660</v>
       </c>
       <c r="L56" s="22"/>
@@ -2138,8 +2140,8 @@
       <c r="H57" t="s">
         <v>61</v>
       </c>
-      <c r="I57" s="31"/>
-      <c r="J57" s="31"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="38"/>
       <c r="L57" s="22"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
@@ -2149,8 +2151,8 @@
       <c r="H58" t="s">
         <v>62</v>
       </c>
-      <c r="I58" s="31"/>
-      <c r="J58" s="31"/>
+      <c r="I58" s="38"/>
+      <c r="J58" s="38"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
@@ -2159,8 +2161,8 @@
       <c r="H59" t="s">
         <v>120</v>
       </c>
-      <c r="I59" s="31"/>
-      <c r="J59" s="31"/>
+      <c r="I59" s="38"/>
+      <c r="J59" s="38"/>
       <c r="L59" s="22"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
@@ -2170,8 +2172,8 @@
       <c r="H60" t="s">
         <v>121</v>
       </c>
-      <c r="I60" s="31"/>
-      <c r="J60" s="31"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="38"/>
       <c r="L60" s="22"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
@@ -2197,10 +2199,10 @@
       <c r="H63" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="I63" s="31">
+      <c r="I63" s="38">
         <v>44664</v>
       </c>
-      <c r="J63" s="31">
+      <c r="J63" s="38">
         <v>44667</v>
       </c>
       <c r="L63" s="22"/>
@@ -2212,8 +2214,8 @@
       <c r="H64" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="I64" s="31"/>
-      <c r="J64" s="31"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
       <c r="L64" s="22"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.35">
@@ -2223,8 +2225,8 @@
       <c r="H65" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="I65" s="31"/>
-      <c r="J65" s="31"/>
+      <c r="I65" s="38"/>
+      <c r="J65" s="38"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="17" t="s">
@@ -2233,8 +2235,8 @@
       <c r="H66" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="I66" s="31"/>
-      <c r="J66" s="31"/>
+      <c r="I66" s="38"/>
+      <c r="J66" s="38"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="17" t="s">
@@ -2243,8 +2245,8 @@
       <c r="H67" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="I67" s="31"/>
-      <c r="J67" s="31"/>
+      <c r="I67" s="38"/>
+      <c r="J67" s="38"/>
       <c r="L67" s="22"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.35">
@@ -2254,8 +2256,8 @@
       <c r="H68" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="I68" s="31"/>
-      <c r="J68" s="31"/>
+      <c r="I68" s="38"/>
+      <c r="J68" s="38"/>
       <c r="L68" s="22"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.35">
@@ -2265,8 +2267,8 @@
       <c r="H69" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="I69" s="31"/>
-      <c r="J69" s="31"/>
+      <c r="I69" s="38"/>
+      <c r="J69" s="38"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="17" t="s">
@@ -2275,8 +2277,8 @@
       <c r="H70" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="I70" s="31"/>
-      <c r="J70" s="31"/>
+      <c r="I70" s="38"/>
+      <c r="J70" s="38"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="17" t="s">
@@ -2285,8 +2287,8 @@
       <c r="H71" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="I71" s="31"/>
-      <c r="J71" s="31"/>
+      <c r="I71" s="38"/>
+      <c r="J71" s="38"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="17" t="s">
@@ -2318,12 +2320,12 @@
       <c r="A75" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B75" s="33" t="s">
+      <c r="B75" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="C75" s="33"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="34"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="35"/>
       <c r="H75" s="10" t="s">
         <v>92</v>
       </c>
@@ -2355,10 +2357,10 @@
       <c r="H78" t="s">
         <v>67</v>
       </c>
-      <c r="I78" s="31">
+      <c r="I78" s="38">
         <v>44671</v>
       </c>
-      <c r="J78" s="31">
+      <c r="J78" s="38">
         <v>44673</v>
       </c>
     </row>
@@ -2372,8 +2374,8 @@
       <c r="H79" t="s">
         <v>68</v>
       </c>
-      <c r="I79" s="31"/>
-      <c r="J79" s="31"/>
+      <c r="I79" s="38"/>
+      <c r="J79" s="38"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="17" t="s">
@@ -2385,8 +2387,8 @@
       <c r="H80" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="I80" s="31"/>
-      <c r="J80" s="31"/>
+      <c r="I80" s="38"/>
+      <c r="J80" s="38"/>
     </row>
     <row r="81" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="17"/>
@@ -2401,12 +2403,12 @@
       <c r="A82" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B82" s="33" t="s">
+      <c r="B82" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="C82" s="33"/>
-      <c r="D82" s="33"/>
-      <c r="E82" s="34"/>
+      <c r="C82" s="34"/>
+      <c r="D82" s="34"/>
+      <c r="E82" s="35"/>
       <c r="H82" s="17" t="s">
         <v>161</v>
       </c>
@@ -2443,10 +2445,10 @@
       <c r="H85" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="I85" s="31">
+      <c r="I85" s="38">
         <v>44676</v>
       </c>
-      <c r="J85" s="31">
+      <c r="J85" s="38">
         <v>44678</v>
       </c>
     </row>
@@ -2454,29 +2456,29 @@
       <c r="H86" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="I86" s="31"/>
-      <c r="J86" s="31"/>
+      <c r="I86" s="38"/>
+      <c r="J86" s="38"/>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H87" t="s">
         <v>69</v>
       </c>
-      <c r="I87" s="31"/>
-      <c r="J87" s="31"/>
+      <c r="I87" s="38"/>
+      <c r="J87" s="38"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H88" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="I88" s="31"/>
-      <c r="J88" s="31"/>
+      <c r="I88" s="38"/>
+      <c r="J88" s="38"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H89" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="I89" s="31"/>
-      <c r="J89" s="31"/>
+      <c r="I89" s="38"/>
+      <c r="J89" s="38"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H90" s="17" t="s">
@@ -2487,10 +2489,10 @@
       <c r="H91" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="I91" s="31">
+      <c r="I91" s="38">
         <v>44679</v>
       </c>
-      <c r="J91" s="31">
+      <c r="J91" s="38">
         <v>44681</v>
       </c>
     </row>
@@ -2498,43 +2500,43 @@
       <c r="H92" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="I92" s="31"/>
-      <c r="J92" s="31"/>
+      <c r="I92" s="38"/>
+      <c r="J92" s="38"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H93" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="I93" s="31"/>
-      <c r="J93" s="31"/>
+      <c r="I93" s="38"/>
+      <c r="J93" s="38"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H94" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="I94" s="31"/>
-      <c r="J94" s="31"/>
+      <c r="I94" s="38"/>
+      <c r="J94" s="38"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H95" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="I95" s="31"/>
-      <c r="J95" s="31"/>
+      <c r="I95" s="38"/>
+      <c r="J95" s="38"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H96" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="I96" s="31"/>
-      <c r="J96" s="31"/>
+      <c r="I96" s="38"/>
+      <c r="J96" s="38"/>
     </row>
     <row r="97" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H97" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="I97" s="31"/>
-      <c r="J97" s="31"/>
+      <c r="I97" s="38"/>
+      <c r="J97" s="38"/>
     </row>
     <row r="98" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H98" s="17" t="s">
@@ -2550,10 +2552,10 @@
       <c r="H100" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="I100" s="31">
+      <c r="I100" s="38">
         <v>44684</v>
       </c>
-      <c r="J100" s="31">
+      <c r="J100" s="38">
         <v>44686</v>
       </c>
     </row>
@@ -2561,52 +2563,52 @@
       <c r="H101" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="I101" s="31"/>
-      <c r="J101" s="31"/>
+      <c r="I101" s="38"/>
+      <c r="J101" s="38"/>
     </row>
     <row r="102" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H102" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="I102" s="31"/>
-      <c r="J102" s="31"/>
+      <c r="I102" s="38"/>
+      <c r="J102" s="38"/>
     </row>
     <row r="103" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H103" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="I103" s="31"/>
-      <c r="J103" s="31"/>
+      <c r="I103" s="38"/>
+      <c r="J103" s="38"/>
     </row>
     <row r="104" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H104" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="I104" s="31"/>
-      <c r="J104" s="31"/>
+      <c r="I104" s="38"/>
+      <c r="J104" s="38"/>
     </row>
     <row r="105" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H105" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="I105" s="31"/>
-      <c r="J105" s="31"/>
+      <c r="I105" s="38"/>
+      <c r="J105" s="38"/>
     </row>
     <row r="106" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H106" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="I106" s="31"/>
-      <c r="J106" s="31"/>
+      <c r="I106" s="38"/>
+      <c r="J106" s="38"/>
     </row>
     <row r="107" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H107" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="I107" s="31">
+      <c r="I107" s="38">
         <v>44687</v>
       </c>
-      <c r="J107" s="31">
+      <c r="J107" s="38">
         <v>44691</v>
       </c>
     </row>
@@ -2614,29 +2616,29 @@
       <c r="H108" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="I108" s="31"/>
-      <c r="J108" s="31"/>
+      <c r="I108" s="38"/>
+      <c r="J108" s="38"/>
     </row>
     <row r="109" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H109" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="I109" s="31"/>
-      <c r="J109" s="31"/>
+      <c r="I109" s="38"/>
+      <c r="J109" s="38"/>
     </row>
     <row r="110" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H110" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="I110" s="31"/>
-      <c r="J110" s="31"/>
+      <c r="I110" s="38"/>
+      <c r="J110" s="38"/>
     </row>
     <row r="111" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H111" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="I111" s="31"/>
-      <c r="J111" s="31"/>
+      <c r="I111" s="38"/>
+      <c r="J111" s="38"/>
     </row>
     <row r="112" spans="8:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="113" spans="8:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2654,10 +2656,10 @@
       <c r="H114" t="s">
         <v>95</v>
       </c>
-      <c r="I114" s="32">
+      <c r="I114" s="39">
         <v>44693</v>
       </c>
-      <c r="J114" s="32">
+      <c r="J114" s="39">
         <v>44695</v>
       </c>
     </row>
@@ -2665,38 +2667,38 @@
       <c r="H115" t="s">
         <v>96</v>
       </c>
-      <c r="I115" s="31"/>
-      <c r="J115" s="31"/>
+      <c r="I115" s="38"/>
+      <c r="J115" s="38"/>
     </row>
     <row r="116" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H116" t="s">
         <v>99</v>
       </c>
-      <c r="I116" s="31"/>
-      <c r="J116" s="31"/>
+      <c r="I116" s="38"/>
+      <c r="J116" s="38"/>
     </row>
     <row r="117" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H117" t="s">
         <v>100</v>
       </c>
-      <c r="I117" s="31"/>
-      <c r="J117" s="31"/>
+      <c r="I117" s="38"/>
+      <c r="J117" s="38"/>
     </row>
     <row r="118" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H118" t="s">
         <v>98</v>
       </c>
-      <c r="I118" s="31"/>
-      <c r="J118" s="31"/>
+      <c r="I118" s="38"/>
+      <c r="J118" s="38"/>
     </row>
     <row r="119" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H119" t="s">
         <v>97</v>
       </c>
-      <c r="I119" s="31">
+      <c r="I119" s="38">
         <v>44699</v>
       </c>
-      <c r="J119" s="31">
+      <c r="J119" s="38">
         <v>44701</v>
       </c>
     </row>
@@ -2704,26 +2706,30 @@
       <c r="H120" t="s">
         <v>194</v>
       </c>
-      <c r="I120" s="31"/>
-      <c r="J120" s="31"/>
+      <c r="I120" s="38"/>
+      <c r="J120" s="38"/>
     </row>
     <row r="121" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H121" t="s">
         <v>195</v>
       </c>
-      <c r="I121" s="31"/>
-      <c r="J121" s="31"/>
+      <c r="I121" s="38"/>
+      <c r="J121" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I31:L31"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="I85:I89"/>
+    <mergeCell ref="J85:J89"/>
+    <mergeCell ref="I114:I118"/>
+    <mergeCell ref="J114:J118"/>
+    <mergeCell ref="I119:I121"/>
+    <mergeCell ref="J119:J121"/>
+    <mergeCell ref="I91:I97"/>
+    <mergeCell ref="J91:J97"/>
+    <mergeCell ref="I100:I106"/>
+    <mergeCell ref="J100:J106"/>
+    <mergeCell ref="I107:I111"/>
+    <mergeCell ref="J107:J111"/>
     <mergeCell ref="B75:E75"/>
     <mergeCell ref="B82:E82"/>
     <mergeCell ref="I41:I44"/>
@@ -2740,18 +2746,14 @@
     <mergeCell ref="I63:I71"/>
     <mergeCell ref="I78:I80"/>
     <mergeCell ref="J78:J80"/>
-    <mergeCell ref="I85:I89"/>
-    <mergeCell ref="J85:J89"/>
-    <mergeCell ref="I114:I118"/>
-    <mergeCell ref="J114:J118"/>
-    <mergeCell ref="I119:I121"/>
-    <mergeCell ref="J119:J121"/>
-    <mergeCell ref="I91:I97"/>
-    <mergeCell ref="J91:J97"/>
-    <mergeCell ref="I100:I106"/>
-    <mergeCell ref="J100:J106"/>
-    <mergeCell ref="I107:I111"/>
-    <mergeCell ref="J107:J111"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I31:L31"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B24:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2788,20 +2790,20 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="H3" s="35" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="H3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="37"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="33"/>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
@@ -3008,18 +3010,18 @@
       <c r="B17" s="42" t="s">
         <v>197</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="35"/>
       <c r="H17" s="10" t="s">
         <v>204</v>
       </c>
       <c r="I17" s="42" t="s">
         <v>197</v>
       </c>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="35"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
@@ -3279,12 +3281,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="I11:L11"/>
     <mergeCell ref="I31:L31"/>
     <mergeCell ref="I35:L35"/>
     <mergeCell ref="B27:E27"/>
@@ -3293,6 +3289,12 @@
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="I17:L17"/>
     <mergeCell ref="I23:L23"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="I11:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add sercice categories use cases and endpoints
</commit_message>
<xml_diff>
--- a/Artisan Backend Timeline.xlsx
+++ b/Artisan Backend Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\locale\ly\projects\artisan-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49C5D43-CC2A-4807-97DD-2C2D10CF97D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0A3426-D801-47BE-BEF2-59D96731C08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7352EEA0-E213-4B45-A5B2-9E24555BD19A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{7352EEA0-E213-4B45-A5B2-9E24555BD19A}"/>
   </bookViews>
   <sheets>
     <sheet name="Artisan Connect" sheetId="2" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="224">
-  <si>
-    <t>Project</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="265">
   <si>
     <t>Tasks</t>
   </si>
@@ -629,66 +626,18 @@
     <t>Administration</t>
   </si>
   <si>
-    <t>Asset Management</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>Staff Registration</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>Residents</t>
-  </si>
-  <si>
     <t>Visitor Logs</t>
   </si>
   <si>
     <t>Email Broadcast</t>
   </si>
   <si>
-    <t xml:space="preserve">Milestone </t>
-  </si>
-  <si>
-    <t>Items</t>
-  </si>
-  <si>
-    <t>Usage</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
-    <t>Procurements</t>
-  </si>
-  <si>
-    <t>CAPEX</t>
-  </si>
-  <si>
-    <t>OPEX</t>
-  </si>
-  <si>
     <t>Petty Cash</t>
   </si>
   <si>
-    <t>Milestone</t>
-  </si>
-  <si>
     <t>Reporting</t>
   </si>
   <si>
-    <t>Dashboard</t>
-  </si>
-  <si>
-    <t>Custom Report</t>
-  </si>
-  <si>
-    <t>Dialy Report</t>
-  </si>
-  <si>
     <t>Project Started on</t>
   </si>
   <si>
@@ -704,17 +653,191 @@
     <t>Pending when we have Azure active account</t>
   </si>
   <si>
-    <t>Database Synchronization</t>
-  </si>
-  <si>
     <t>Project Start Date:</t>
+  </si>
+  <si>
+    <t>scaffolding</t>
+  </si>
+  <si>
+    <t>Login Screen</t>
+  </si>
+  <si>
+    <t>Register Screen</t>
+  </si>
+  <si>
+    <t>Forget password</t>
+  </si>
+  <si>
+    <t>Infrastucture</t>
+  </si>
+  <si>
+    <t>Model Design</t>
+  </si>
+  <si>
+    <t>Application Logic</t>
+  </si>
+  <si>
+    <t>Secret storage</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Create House</t>
+  </si>
+  <si>
+    <t>House Screen</t>
+  </si>
+  <si>
+    <t>Delete House</t>
+  </si>
+  <si>
+    <t>Add Resident</t>
+  </si>
+  <si>
+    <t>Remove Resident</t>
+  </si>
+  <si>
+    <t>House domain models</t>
+  </si>
+  <si>
+    <t>Resident models</t>
+  </si>
+  <si>
+    <t>Business logic</t>
+  </si>
+  <si>
+    <t>Database Schema</t>
+  </si>
+  <si>
+    <t>Database design (ERD)</t>
+  </si>
+  <si>
+    <t>Database Syncronization</t>
+  </si>
+  <si>
+    <t>Data import and export</t>
+  </si>
+  <si>
+    <t>Maintenance and Service Charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module 1 </t>
+  </si>
+  <si>
+    <t>Module 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module 3 </t>
+  </si>
+  <si>
+    <t>Module 4</t>
+  </si>
+  <si>
+    <t>Module 5</t>
+  </si>
+  <si>
+    <t>Module 6</t>
+  </si>
+  <si>
+    <t>Table Screen</t>
+  </si>
+  <si>
+    <t>Add Credit</t>
+  </si>
+  <si>
+    <t>Add Debit</t>
+  </si>
+  <si>
+    <t>Remove Record</t>
+  </si>
+  <si>
+    <t>Input Validation</t>
+  </si>
+  <si>
+    <t>Data validation</t>
+  </si>
+  <si>
+    <t>Email implemenation</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Invoice Table</t>
+  </si>
+  <si>
+    <t>Create Invoice</t>
+  </si>
+  <si>
+    <t>Consume Payment API</t>
+  </si>
+  <si>
+    <t>Dialy Invoice Table</t>
+  </si>
+  <si>
+    <t>Dialy Payment Table</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Power Usage Table</t>
+  </si>
+  <si>
+    <t>Create Generator</t>
+  </si>
+  <si>
+    <t>Delete Generator</t>
+  </si>
+  <si>
+    <t>On Generator</t>
+  </si>
+  <si>
+    <t>Off Generator</t>
+  </si>
+  <si>
+    <t>On PHCN</t>
+  </si>
+  <si>
+    <t>Off PHCN</t>
+  </si>
+  <si>
+    <t>Delete Power Usage</t>
+  </si>
+  <si>
+    <t>Update Power Usage</t>
+  </si>
+  <si>
+    <t>Module 7</t>
+  </si>
+  <si>
+    <t>Attendance</t>
+  </si>
+  <si>
+    <t>User Screen</t>
+  </si>
+  <si>
+    <t>Attendance Table</t>
+  </si>
+  <si>
+    <t>Add Sign in</t>
+  </si>
+  <si>
+    <t>Add Sign out</t>
+  </si>
+  <si>
+    <t>API Design &amp; Development</t>
+  </si>
+  <si>
+    <t>Analytics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -745,8 +868,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -795,8 +925,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -873,37 +1015,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -967,60 +1078,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1032,32 +1111,49 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1066,19 +1162,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1397,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EC11CA-85A1-4736-9D8D-54DA1C1DECD6}">
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E43" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView topLeftCell="E22" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1417,7 +1504,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.5">
       <c r="F1" s="2" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="G1" s="3">
         <v>44612</v>
@@ -1427,435 +1514,435 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="44"/>
+      <c r="H3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="H3" s="31" t="s">
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="44"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="33"/>
-    </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="34" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="H4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="35"/>
-      <c r="H4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="35"/>
+      <c r="I4" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="41"/>
       <c r="N4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="46"/>
+      <c r="D5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="46"/>
+      <c r="K5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="L5" t="s">
-        <v>51</v>
-      </c>
-      <c r="O5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5"/>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>16</v>
       </c>
       <c r="D6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="16" t="s">
-        <v>16</v>
-      </c>
       <c r="K6" s="5"/>
-      <c r="N6" s="20"/>
+      <c r="N6" s="16"/>
       <c r="O6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="H7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="20"/>
-      <c r="N7" s="19"/>
+      <c r="L7" s="16"/>
+      <c r="N7" s="15"/>
       <c r="O7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="H8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="20"/>
-      <c r="N8" s="18"/>
+      <c r="L8" s="16"/>
+      <c r="N8" s="14"/>
       <c r="O8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="H9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="L9" s="19"/>
+        <v>90</v>
+      </c>
+      <c r="L9" s="15"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="H10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="20"/>
+      <c r="L10" s="16"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="H11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="20"/>
+      <c r="L11" s="16"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="H12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="20"/>
+      <c r="L12" s="16"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="H13" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="20"/>
+      <c r="L13" s="16"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="H14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="20"/>
+      <c r="L14" s="16"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="H15" s="17" t="s">
-        <v>32</v>
+      <c r="H15" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="L15" s="20"/>
+      <c r="L15" s="16"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="H16" s="17" t="s">
-        <v>10</v>
+      <c r="H16" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-      <c r="L16" s="20"/>
+      <c r="L16" s="16"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="H17" s="17" t="s">
-        <v>14</v>
+      <c r="H17" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="L17" s="20"/>
+      <c r="L17" s="16"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="17" t="s">
-        <v>88</v>
+      <c r="A18" s="13" t="s">
+        <v>87</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="19"/>
-      <c r="H18" s="17" t="s">
-        <v>33</v>
+      <c r="E18" s="15"/>
+      <c r="H18" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="L18" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="L18" s="15"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H20" s="13" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="17" t="s">
+      <c r="L20" s="16"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="16"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="H20" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="L20" s="20"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="H21" s="17" t="s">
+      <c r="H22" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="L21" s="20"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="H22" s="17" t="s">
+      <c r="L22" s="16"/>
+    </row>
+    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H23" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="L22" s="20"/>
-    </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H23" s="17" t="s">
+      <c r="L23" s="16"/>
+    </row>
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="41"/>
+      <c r="H24" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="L23" s="20"/>
-    </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="35"/>
-      <c r="H24" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="L24" s="20"/>
+      <c r="L24" s="16"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="H25" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="L25" s="18"/>
+      <c r="H25" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="L25" s="14"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="H26" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L26" s="22"/>
+      <c r="H26" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="18"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="H27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="L27" s="20"/>
+        <v>41</v>
+      </c>
+      <c r="L27" s="16"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="L28" s="23"/>
+      <c r="A28" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="L28" s="19"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A29" s="17" t="s">
-        <v>54</v>
+      <c r="A29" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="L29" s="21"/>
+        <v>48</v>
+      </c>
+      <c r="L29" s="17"/>
     </row>
     <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="17" t="s">
-        <v>55</v>
+      <c r="A30" s="13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I31" s="34" t="s">
+      <c r="A31" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="41"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32" t="s">
         <v>57</v>
       </c>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="35"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32" s="17" t="s">
+      <c r="K32" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H32" t="s">
-        <v>58</v>
-      </c>
-      <c r="K32" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A33" s="17" t="s">
-        <v>72</v>
-      </c>
       <c r="H33" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I33" s="1">
         <v>44634</v>
@@ -1864,25 +1951,25 @@
         <v>44636</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="L33" s="22"/>
+        <v>203</v>
+      </c>
+      <c r="L33" s="18"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="H34" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K34" s="5"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A35" s="17" t="s">
-        <v>75</v>
-      </c>
       <c r="H35" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I35" s="1">
         <v>44639</v>
@@ -1890,68 +1977,68 @@
       <c r="J35" s="1">
         <v>44639</v>
       </c>
-      <c r="L35" s="22"/>
+      <c r="L35" s="18"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="K36" s="5"/>
+      <c r="L36" s="14"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A37" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H36" s="17" t="s">
+      <c r="H37" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="K36" s="5"/>
-      <c r="L36" s="18"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A37" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="H37" s="17" t="s">
+      <c r="K37" s="5"/>
+      <c r="L37" s="14"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A38" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="K37" s="5"/>
-      <c r="L37" s="18"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A38" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="H38" s="17" t="s">
+      <c r="H38" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="D39" t="s">
+        <v>168</v>
+      </c>
+      <c r="H39" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="K38" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A39" s="17" t="s">
+      <c r="K39" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="L39" s="18"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="D39" t="s">
-        <v>169</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="L39" s="22"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A40" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="H40" s="17" t="s">
-        <v>111</v>
+      <c r="H40" s="13" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A41" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>123</v>
+      <c r="A41" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>122</v>
       </c>
       <c r="I41" s="38">
         <v>44641</v>
@@ -1959,48 +2046,50 @@
       <c r="J41" s="38">
         <v>44642</v>
       </c>
-      <c r="L41" s="22"/>
+      <c r="L41" s="18"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A42" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="H42" s="17" t="s">
-        <v>113</v>
+      <c r="A42" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="I42" s="38"/>
       <c r="J42" s="38"/>
-      <c r="L42" s="22"/>
+      <c r="L42" s="18"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A43" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="H43" s="17" t="s">
-        <v>114</v>
+      <c r="A43" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="I43" s="38"/>
       <c r="J43" s="38"/>
+      <c r="L43" s="18"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A44" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="H44" s="17" t="s">
-        <v>115</v>
+      <c r="A44" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="I44" s="38"/>
       <c r="J44" s="38"/>
+      <c r="L44" s="14"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A45" s="17" t="s">
-        <v>167</v>
+      <c r="A45" s="13" t="s">
+        <v>166</v>
       </c>
       <c r="D45" t="s">
-        <v>169</v>
-      </c>
-      <c r="H45" s="17" t="s">
-        <v>124</v>
+        <v>168</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="I45" s="38">
         <v>44644</v>
@@ -2008,45 +2097,46 @@
       <c r="J45" s="38">
         <v>44645</v>
       </c>
-      <c r="L45" s="22"/>
+      <c r="L45" s="18"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A46" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="H46" s="17" t="s">
-        <v>125</v>
+      <c r="A46" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="I46" s="38"/>
       <c r="J46" s="38"/>
-      <c r="L46" s="22"/>
+      <c r="L46" s="18"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A47" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="H47" s="17" t="s">
-        <v>126</v>
+      <c r="A47" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>125</v>
       </c>
       <c r="I47" s="38"/>
       <c r="J47" s="38"/>
+      <c r="L47" s="18"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A48" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="H48" s="17" t="s">
-        <v>127</v>
+      <c r="A48" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="I48" s="38"/>
       <c r="J48" s="38"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A49" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="H49" s="17" t="s">
-        <v>112</v>
+      <c r="A49" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="I49" s="38">
         <v>44646</v>
@@ -2056,29 +2146,29 @@
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A50" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H50" s="17" t="s">
-        <v>116</v>
+      <c r="A50" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="I50" s="38"/>
       <c r="J50" s="38"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="H51" s="17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A52" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="H52" s="17" t="s">
-        <v>117</v>
+      <c r="H52" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="I52" s="38">
         <v>44652</v>
@@ -2086,44 +2176,46 @@
       <c r="J52" s="38">
         <v>44655</v>
       </c>
+      <c r="L52" s="18"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A53" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="H53" s="17" t="s">
-        <v>118</v>
+      <c r="A53" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="I53" s="38"/>
       <c r="J53" s="38"/>
+      <c r="L53" s="18"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A54" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="H54" s="17" t="s">
-        <v>119</v>
+      <c r="A54" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="I54" s="38"/>
       <c r="J54" s="38"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="H55" t="s">
+        <v>58</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A56" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H56" t="s">
         <v>59</v>
-      </c>
-      <c r="K55" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A56" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="H56" t="s">
-        <v>60</v>
       </c>
       <c r="I56" s="38">
         <v>44657</v>
@@ -2131,73 +2223,73 @@
       <c r="J56" s="38">
         <v>44660</v>
       </c>
-      <c r="L56" s="22"/>
+      <c r="L56" s="18"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A57" s="17" t="s">
-        <v>104</v>
+      <c r="A57" s="13" t="s">
+        <v>103</v>
       </c>
       <c r="H57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I57" s="38"/>
       <c r="J57" s="38"/>
-      <c r="L57" s="22"/>
+      <c r="L57" s="18"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A58" s="17" t="s">
-        <v>105</v>
+      <c r="A58" s="13" t="s">
+        <v>104</v>
       </c>
       <c r="H58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I58" s="38"/>
       <c r="J58" s="38"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A59" s="17" t="s">
-        <v>106</v>
+      <c r="A59" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="H59" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I59" s="38"/>
       <c r="J59" s="38"/>
-      <c r="L59" s="22"/>
+      <c r="L59" s="18"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A60" s="17" t="s">
-        <v>88</v>
+      <c r="A60" s="13" t="s">
+        <v>87</v>
       </c>
       <c r="H60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I60" s="38"/>
       <c r="J60" s="38"/>
-      <c r="L60" s="22"/>
+      <c r="L60" s="18"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A61" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="H61" s="17" t="s">
+      <c r="A61" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A62" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="H62" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A62" s="17" t="s">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A63" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="H62" s="17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A63" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="H63" s="17" t="s">
-        <v>128</v>
+      <c r="H63" s="13" t="s">
+        <v>127</v>
       </c>
       <c r="I63" s="38">
         <v>44664</v>
@@ -2205,157 +2297,160 @@
       <c r="J63" s="38">
         <v>44667</v>
       </c>
-      <c r="L63" s="22"/>
+      <c r="L63" s="18"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A64" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="H64" s="17" t="s">
-        <v>129</v>
+      <c r="A64" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="H64" s="13" t="s">
+        <v>128</v>
       </c>
       <c r="I64" s="38"/>
       <c r="J64" s="38"/>
-      <c r="L64" s="22"/>
+      <c r="L64" s="18"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A65" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="H65" s="17" t="s">
-        <v>130</v>
+      <c r="A65" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>129</v>
       </c>
       <c r="I65" s="38"/>
       <c r="J65" s="38"/>
+      <c r="L65" s="18"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A66" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="H66" s="17" t="s">
-        <v>131</v>
+      <c r="A66" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="H66" s="13" t="s">
+        <v>130</v>
       </c>
       <c r="I66" s="38"/>
       <c r="J66" s="38"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A67" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="H67" s="17" t="s">
-        <v>132</v>
+      <c r="A67" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="H67" s="13" t="s">
+        <v>131</v>
       </c>
       <c r="I67" s="38"/>
       <c r="J67" s="38"/>
-      <c r="L67" s="22"/>
+      <c r="L67" s="18"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A68" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="H68" s="17" t="s">
-        <v>133</v>
+      <c r="A68" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="H68" s="13" t="s">
+        <v>132</v>
       </c>
       <c r="I68" s="38"/>
       <c r="J68" s="38"/>
-      <c r="L68" s="22"/>
+      <c r="L68" s="18"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A69" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="H69" s="17" t="s">
-        <v>134</v>
+      <c r="A69" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="H69" s="13" t="s">
+        <v>133</v>
       </c>
       <c r="I69" s="38"/>
       <c r="J69" s="38"/>
+      <c r="L69" s="18"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A70" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="H70" s="17" t="s">
-        <v>135</v>
+      <c r="A70" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="H70" s="13" t="s">
+        <v>134</v>
       </c>
       <c r="I70" s="38"/>
       <c r="J70" s="38"/>
+      <c r="L70" s="14"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A71" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="H71" s="17" t="s">
-        <v>136</v>
+      <c r="A71" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="H71" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="I71" s="38"/>
       <c r="J71" s="38"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A72" s="17" t="s">
+      <c r="A72" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="H72" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="I72" s="23"/>
+      <c r="K72" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="L72" s="18"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A73" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="H72" s="17" t="s">
+      <c r="H73" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="I72" s="30"/>
-      <c r="K72" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="L72" s="22"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A73" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="H73" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="I73" s="30"/>
+      <c r="I73" s="23"/>
       <c r="K73" s="5" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="75" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B75" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="C75" s="34"/>
-      <c r="D75" s="34"/>
-      <c r="E75" s="35"/>
-      <c r="H75" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="I75" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="J75" s="24"/>
-      <c r="K75" s="24"/>
-      <c r="L75" s="25"/>
+      <c r="A75" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B75" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="C75" s="40"/>
+      <c r="D75" s="40"/>
+      <c r="E75" s="41"/>
+      <c r="H75" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I75" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="J75" s="20"/>
+      <c r="K75" s="20"/>
+      <c r="L75" s="21"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D77" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H77" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D78" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H78" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I78" s="38">
         <v>44671</v>
@@ -2366,84 +2461,84 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
+        <v>151</v>
+      </c>
+      <c r="D79" t="s">
         <v>152</v>
       </c>
-      <c r="D79" t="s">
-        <v>153</v>
-      </c>
       <c r="H79" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I79" s="38"/>
       <c r="J79" s="38"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A80" s="17" t="s">
-        <v>155</v>
+      <c r="A80" s="13" t="s">
+        <v>154</v>
       </c>
       <c r="D80" t="s">
-        <v>154</v>
-      </c>
-      <c r="H80" s="17" t="s">
-        <v>157</v>
+        <v>153</v>
+      </c>
+      <c r="H80" s="13" t="s">
+        <v>156</v>
       </c>
       <c r="I80" s="38"/>
       <c r="J80" s="38"/>
     </row>
     <row r="81" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="17"/>
-      <c r="H81" s="17" t="s">
+      <c r="A81" s="13"/>
+      <c r="H81" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="K81" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B82" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="C82" s="40"/>
+      <c r="D82" s="40"/>
+      <c r="E82" s="41"/>
+      <c r="H82" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="K81" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B82" s="34" t="s">
-        <v>213</v>
-      </c>
-      <c r="C82" s="34"/>
-      <c r="D82" s="34"/>
-      <c r="E82" s="35"/>
-      <c r="H82" s="17" t="s">
+      <c r="K82" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="L82" s="18"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H83" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="K82" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="L82" s="22"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H83" s="17" t="s">
-        <v>162</v>
-      </c>
       <c r="K83" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="L83" s="22"/>
+        <v>204</v>
+      </c>
+      <c r="L83" s="18"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="D84" t="s">
-        <v>219</v>
-      </c>
-      <c r="H84" s="17" t="s">
-        <v>163</v>
+        <v>202</v>
+      </c>
+      <c r="H84" s="13" t="s">
+        <v>162</v>
       </c>
       <c r="K84" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="L84" s="22"/>
+        <v>204</v>
+      </c>
+      <c r="L84" s="18"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H85" s="17" t="s">
-        <v>166</v>
+      <c r="H85" s="13" t="s">
+        <v>165</v>
       </c>
       <c r="I85" s="38">
         <v>44676</v>
@@ -2453,41 +2548,41 @@
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H86" s="17" t="s">
-        <v>170</v>
+      <c r="H86" s="13" t="s">
+        <v>169</v>
       </c>
       <c r="I86" s="38"/>
       <c r="J86" s="38"/>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I87" s="38"/>
       <c r="J87" s="38"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H88" s="17" t="s">
-        <v>164</v>
+      <c r="H88" s="13" t="s">
+        <v>163</v>
       </c>
       <c r="I88" s="38"/>
       <c r="J88" s="38"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H89" s="17" t="s">
-        <v>165</v>
+      <c r="H89" s="13" t="s">
+        <v>164</v>
       </c>
       <c r="I89" s="38"/>
       <c r="J89" s="38"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H90" s="17" t="s">
+      <c r="H90" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H91" s="13" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H91" s="17" t="s">
-        <v>174</v>
       </c>
       <c r="I91" s="38">
         <v>44679</v>
@@ -2497,60 +2592,60 @@
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H92" s="17" t="s">
-        <v>175</v>
+      <c r="H92" s="13" t="s">
+        <v>174</v>
       </c>
       <c r="I92" s="38"/>
       <c r="J92" s="38"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H93" s="17" t="s">
-        <v>176</v>
+      <c r="H93" s="13" t="s">
+        <v>175</v>
       </c>
       <c r="I93" s="38"/>
       <c r="J93" s="38"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H94" s="17" t="s">
-        <v>177</v>
+      <c r="H94" s="13" t="s">
+        <v>176</v>
       </c>
       <c r="I94" s="38"/>
       <c r="J94" s="38"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H95" s="17" t="s">
-        <v>178</v>
+      <c r="H95" s="13" t="s">
+        <v>177</v>
       </c>
       <c r="I95" s="38"/>
       <c r="J95" s="38"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H96" s="17" t="s">
-        <v>179</v>
+      <c r="H96" s="13" t="s">
+        <v>178</v>
       </c>
       <c r="I96" s="38"/>
       <c r="J96" s="38"/>
     </row>
     <row r="97" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H97" s="17" t="s">
-        <v>180</v>
+      <c r="H97" s="13" t="s">
+        <v>179</v>
       </c>
       <c r="I97" s="38"/>
       <c r="J97" s="38"/>
     </row>
     <row r="98" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H98" s="17" t="s">
-        <v>33</v>
+      <c r="H98" s="13" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="99" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H99" s="17" t="s">
+      <c r="H99" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="100" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H100" s="13" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="100" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H100" s="17" t="s">
-        <v>182</v>
       </c>
       <c r="I100" s="38">
         <v>44684</v>
@@ -2560,50 +2655,50 @@
       </c>
     </row>
     <row r="101" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H101" s="17" t="s">
-        <v>183</v>
+      <c r="H101" s="13" t="s">
+        <v>182</v>
       </c>
       <c r="I101" s="38"/>
       <c r="J101" s="38"/>
     </row>
     <row r="102" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H102" s="17" t="s">
-        <v>184</v>
+      <c r="H102" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="I102" s="38"/>
       <c r="J102" s="38"/>
     </row>
     <row r="103" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H103" s="17" t="s">
-        <v>185</v>
+      <c r="H103" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="I103" s="38"/>
       <c r="J103" s="38"/>
     </row>
     <row r="104" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H104" s="17" t="s">
-        <v>186</v>
+      <c r="H104" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="I104" s="38"/>
       <c r="J104" s="38"/>
     </row>
     <row r="105" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H105" s="17" t="s">
-        <v>187</v>
+      <c r="H105" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="I105" s="38"/>
       <c r="J105" s="38"/>
     </row>
     <row r="106" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H106" s="17" t="s">
-        <v>188</v>
+      <c r="H106" s="13" t="s">
+        <v>187</v>
       </c>
       <c r="I106" s="38"/>
       <c r="J106" s="38"/>
     </row>
     <row r="107" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H107" s="17" t="s">
-        <v>189</v>
+      <c r="H107" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="I107" s="38">
         <v>44687</v>
@@ -2613,48 +2708,48 @@
       </c>
     </row>
     <row r="108" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H108" s="17" t="s">
-        <v>190</v>
+      <c r="H108" s="13" t="s">
+        <v>189</v>
       </c>
       <c r="I108" s="38"/>
       <c r="J108" s="38"/>
     </row>
     <row r="109" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H109" s="17" t="s">
-        <v>191</v>
+      <c r="H109" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="I109" s="38"/>
       <c r="J109" s="38"/>
     </row>
     <row r="110" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H110" s="17" t="s">
-        <v>192</v>
+      <c r="H110" s="13" t="s">
+        <v>191</v>
       </c>
       <c r="I110" s="38"/>
       <c r="J110" s="38"/>
     </row>
     <row r="111" spans="8:10" x14ac:dyDescent="0.35">
-      <c r="H111" s="17" t="s">
-        <v>193</v>
+      <c r="H111" s="13" t="s">
+        <v>192</v>
       </c>
       <c r="I111" s="38"/>
       <c r="J111" s="38"/>
     </row>
     <row r="112" spans="8:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="113" spans="8:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H113" s="10" t="s">
+      <c r="H113" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I113" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="I113" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="J113" s="24"/>
-      <c r="K113" s="24"/>
-      <c r="L113" s="25"/>
+      <c r="J113" s="20"/>
+      <c r="K113" s="20"/>
+      <c r="L113" s="21"/>
     </row>
     <row r="114" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H114" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I114" s="39">
         <v>44693</v>
@@ -2665,35 +2760,35 @@
     </row>
     <row r="115" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H115" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I115" s="38"/>
       <c r="J115" s="38"/>
     </row>
     <row r="116" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H116" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I116" s="38"/>
       <c r="J116" s="38"/>
     </row>
     <row r="117" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H117" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I117" s="38"/>
       <c r="J117" s="38"/>
     </row>
     <row r="118" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H118" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I118" s="38"/>
       <c r="J118" s="38"/>
     </row>
     <row r="119" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H119" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I119" s="38">
         <v>44699</v>
@@ -2704,32 +2799,28 @@
     </row>
     <row r="120" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H120" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I120" s="38"/>
       <c r="J120" s="38"/>
     </row>
     <row r="121" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H121" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I121" s="38"/>
       <c r="J121" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="I85:I89"/>
-    <mergeCell ref="J85:J89"/>
-    <mergeCell ref="I114:I118"/>
-    <mergeCell ref="J114:J118"/>
-    <mergeCell ref="I119:I121"/>
-    <mergeCell ref="J119:J121"/>
-    <mergeCell ref="I91:I97"/>
-    <mergeCell ref="J91:J97"/>
-    <mergeCell ref="I100:I106"/>
-    <mergeCell ref="J100:J106"/>
-    <mergeCell ref="I107:I111"/>
-    <mergeCell ref="J107:J111"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I31:L31"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B24:E24"/>
     <mergeCell ref="B75:E75"/>
     <mergeCell ref="B82:E82"/>
     <mergeCell ref="I41:I44"/>
@@ -2746,14 +2837,18 @@
     <mergeCell ref="I63:I71"/>
     <mergeCell ref="I78:I80"/>
     <mergeCell ref="J78:J80"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I31:L31"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="I85:I89"/>
+    <mergeCell ref="J85:J89"/>
+    <mergeCell ref="I114:I118"/>
+    <mergeCell ref="J114:J118"/>
+    <mergeCell ref="I119:I121"/>
+    <mergeCell ref="J119:J121"/>
+    <mergeCell ref="I91:I97"/>
+    <mergeCell ref="J91:J97"/>
+    <mergeCell ref="I100:I106"/>
+    <mergeCell ref="J100:J106"/>
+    <mergeCell ref="I107:I111"/>
+    <mergeCell ref="J107:J111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2762,25 +2857,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D69E8F-168F-423E-8A0A-90A49C415639}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.5">
       <c r="E1" s="2" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="G1" s="3">
         <v>44608</v>
@@ -2790,511 +2885,885 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="44"/>
+      <c r="H3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="H3" s="31" t="s">
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="44"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="33"/>
-    </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
-      <c r="H4" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="I4" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="41"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="48"/>
+      <c r="H4" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="I4" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="48"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
-      <c r="B5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>3</v>
+      <c r="E5" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="11" t="s">
+      <c r="I5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="11" t="s">
-        <v>3</v>
+      <c r="L5" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="A6" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="25"/>
+      <c r="H6" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+      <c r="A7" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="25"/>
+      <c r="H7" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
+      <c r="A8" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="25"/>
+      <c r="H8" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="30"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
+      <c r="A9" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="30"/>
+      <c r="H9" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="30"/>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="H10" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="30"/>
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
-      <c r="H11" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="I11" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="41"/>
+      <c r="A11" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48"/>
+      <c r="H11" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="I11" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="48"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="15"/>
+        <v>216</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="26"/>
+      <c r="H12" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="26"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
-      <c r="H13" s="4"/>
+      <c r="E13" s="27"/>
+      <c r="H13" s="4" t="s">
+        <v>221</v>
+      </c>
       <c r="I13" s="4"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="6"/>
+      <c r="L13" s="27"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
-      <c r="H14" s="4"/>
+      <c r="E14" s="28"/>
+      <c r="H14" s="4" t="s">
+        <v>222</v>
+      </c>
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="6"/>
+      <c r="L14" s="29"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
-      <c r="H15" s="4"/>
+      <c r="E15" s="27"/>
+      <c r="H15" s="24" t="s">
+        <v>239</v>
+      </c>
       <c r="I15" s="4"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="4" t="s">
-        <v>203</v>
+      <c r="L15" s="28"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="24" t="s">
+        <v>219</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="H16" s="4"/>
+      <c r="E16" s="27"/>
+      <c r="H16" s="24" t="s">
+        <v>226</v>
+      </c>
       <c r="I16" s="4"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="B17" s="42" t="s">
-        <v>197</v>
-      </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
-      <c r="H17" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="I17" s="42" t="s">
-        <v>197</v>
-      </c>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="35"/>
+      <c r="L16" s="29"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="27"/>
+      <c r="H17" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="29"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="H18" s="4"/>
+      <c r="E18" s="28"/>
+      <c r="H18" s="4" t="s">
+        <v>223</v>
+      </c>
       <c r="I18" s="4"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="6"/>
+      <c r="L18" s="29"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>206</v>
-      </c>
+      <c r="A19" s="5"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-      <c r="H19" s="4"/>
+      <c r="E19" s="31"/>
+      <c r="H19" s="4" t="s">
+        <v>225</v>
+      </c>
       <c r="I19" s="4"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="6"/>
+      <c r="L19" s="29"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
-        <v>207</v>
-      </c>
+      <c r="A20" s="5"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-      <c r="H20" s="4"/>
+      <c r="E20" s="31"/>
+      <c r="H20" s="32" t="s">
+        <v>263</v>
+      </c>
       <c r="I20" s="4"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="6"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
-        <v>208</v>
-      </c>
+      <c r="L20" s="29"/>
+    </row>
+    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="H21" s="4"/>
+      <c r="E21" s="31"/>
+      <c r="H21" s="24" t="s">
+        <v>240</v>
+      </c>
       <c r="I21" s="4"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="6"/>
+      <c r="L21" s="29"/>
     </row>
     <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="9"/>
-    </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>198</v>
-      </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="41"/>
-      <c r="H23" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="I23" s="40" t="s">
-        <v>198</v>
-      </c>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="41"/>
+      <c r="A22" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="41"/>
+      <c r="H22" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="I22" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="41"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="27"/>
+      <c r="H23" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="27"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="27" t="s">
-        <v>209</v>
-      </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="15"/>
+      <c r="A24" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="27"/>
+      <c r="H24" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="27"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A25" s="28" t="s">
-        <v>210</v>
-      </c>
-      <c r="B25" s="5"/>
+      <c r="A25" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="5"/>
+      <c r="E25" s="27"/>
+      <c r="H25" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="I25" s="4"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="6"/>
-    </row>
-    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="29" t="s">
+      <c r="L25" s="29"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="27"/>
+      <c r="H26" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="29"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="27"/>
+      <c r="H27" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="29"/>
+    </row>
+    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="27"/>
+      <c r="H28" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="29"/>
+    </row>
+    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="41"/>
+      <c r="H29" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="I29" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="41"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="27"/>
+      <c r="H30" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="9"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="9"/>
-    </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="B27" s="40" t="s">
-        <v>213</v>
-      </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
-      <c r="H27" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="I27" s="40" t="s">
-        <v>213</v>
-      </c>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="41"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="15"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="15"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A29" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="6"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="6"/>
-    </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="29" t="s">
-        <v>216</v>
-      </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="9"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="9"/>
-    </row>
-    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H31" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="I31" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="41"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="27"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="27"/>
+      <c r="H31" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="27"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="H32" s="27"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="15"/>
-    </row>
-    <row r="33" spans="8:12" x14ac:dyDescent="0.35">
-      <c r="H33" s="28"/>
+      <c r="A32" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="27"/>
+      <c r="H32" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="29"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="27"/>
+      <c r="H33" s="4" t="s">
+        <v>224</v>
+      </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="6"/>
-    </row>
-    <row r="34" spans="8:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H34" s="29"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="9"/>
-    </row>
-    <row r="35" spans="8:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H35" s="26" t="s">
-        <v>212</v>
+      <c r="L33" s="29"/>
+    </row>
+    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="27"/>
+      <c r="H34" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="29"/>
+    </row>
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="41"/>
+      <c r="H35" s="6" t="s">
+        <v>232</v>
       </c>
       <c r="I35" s="40" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="J35" s="40"/>
       <c r="K35" s="40"/>
       <c r="L35" s="41"/>
     </row>
-    <row r="36" spans="8:12" x14ac:dyDescent="0.35">
-      <c r="H36" s="27"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="15"/>
-    </row>
-    <row r="37" spans="8:12" x14ac:dyDescent="0.35">
-      <c r="H37" s="28"/>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A36" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="28"/>
+      <c r="H36" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="29"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A37" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="33"/>
+      <c r="H37" s="4" t="s">
+        <v>222</v>
+      </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="6"/>
-    </row>
-    <row r="38" spans="8:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H38" s="29"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="9"/>
+      <c r="L37" s="29"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="29"/>
+      <c r="H38" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="29"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="27"/>
+      <c r="H39" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="29"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="33"/>
+      <c r="H40" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="36"/>
+    </row>
+    <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="13"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="33"/>
+      <c r="H41" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="29"/>
+    </row>
+    <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B42" s="40" t="s">
+        <v>247</v>
+      </c>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="41"/>
+      <c r="H42" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="I42" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="J42" s="47"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="48"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="27"/>
+      <c r="H43" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="27"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="27"/>
+      <c r="H44" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="27"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="29"/>
+      <c r="H45" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="27"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="27"/>
+      <c r="H46" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="29"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="35"/>
+      <c r="H47" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="36"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A48" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E48" s="34"/>
+      <c r="H48" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="L48" s="37"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="E49" s="34"/>
+      <c r="H49" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="E50" s="14"/>
+    </row>
+    <row r="51" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="E51" s="14"/>
+      <c r="H51" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="I51" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="J51" s="40"/>
+      <c r="K51" s="40"/>
+      <c r="L51" s="41"/>
+    </row>
+    <row r="52" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H52" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="26"/>
+    </row>
+    <row r="53" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B53" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="41"/>
+      <c r="H53" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="27"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>259</v>
+      </c>
+      <c r="E54" s="34"/>
+      <c r="H54" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="27"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>260</v>
+      </c>
+      <c r="E55" s="34"/>
+      <c r="H55" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="36"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>261</v>
+      </c>
+      <c r="E56" s="34"/>
+      <c r="H56" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="L56" s="14"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>262</v>
+      </c>
+      <c r="E57" s="34"/>
+      <c r="H57" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="L57" s="14"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H58" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="L58" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="I31:L31"/>
-    <mergeCell ref="I35:L35"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="I23:L23"/>
+  <mergeCells count="16">
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="I11:L11"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="I22:L22"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="I51:L51"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="I35:L35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>